<commit_message>
Sprint Plan & Burndown Chart
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -59,6 +59,51 @@
   </si>
   <si>
     <t>Days</t>
+  </si>
+  <si>
+    <t>Update MSQI Chart</t>
+  </si>
+  <si>
+    <t>Basement Room D: Assets &amp; Props</t>
+  </si>
+  <si>
+    <t>Basement Room B: Assets &amp; Props</t>
+  </si>
+  <si>
+    <t>Basement Room C: Assets &amp; Props</t>
+  </si>
+  <si>
+    <t>Basement Room E: Assets &amp; Props</t>
+  </si>
+  <si>
+    <t>Basement Room F: Assets &amp; Props</t>
+  </si>
+  <si>
+    <t>Room Allocation System</t>
+  </si>
+  <si>
+    <t>AI Patrolling</t>
+  </si>
+  <si>
+    <t>Basement Room A: Event</t>
+  </si>
+  <si>
+    <t>Basement Room B: Event</t>
+  </si>
+  <si>
+    <t>Basement Room D: Event</t>
+  </si>
+  <si>
+    <t>Basement Room E: Event</t>
+  </si>
+  <si>
+    <t>Basement Room F: Event</t>
+  </si>
+  <si>
+    <t>Interaction Diagram (Final Event)</t>
+  </si>
+  <si>
+    <t>User Stories (Final Event)</t>
   </si>
 </sst>
 </file>
@@ -329,19 +374,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -393,22 +438,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,7 +1520,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,27 +1560,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1546,23 +1591,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1597,9 +1642,11 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -1620,9 +1667,11 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -1643,9 +1692,11 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -1666,12 +1717,14 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="B10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="8">
         <v>0</v>
@@ -1689,9 +1742,11 @@
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="B11" s="8">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -1712,9 +1767,11 @@
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -1735,9 +1792,11 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -1758,9 +1817,11 @@
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C14" s="8">
         <v>0</v>
@@ -1781,12 +1842,14 @@
       <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="B15" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="8">
         <v>0</v>
@@ -1804,9 +1867,11 @@
       <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
@@ -1827,9 +1892,11 @@
       <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="B17" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -1850,9 +1917,11 @@
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="B18" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -1873,9 +1942,11 @@
       <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -1896,9 +1967,11 @@
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -1919,9 +1992,11 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Meeting Recording & Burndown Update
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD06AF-A96A-4DB9-94CF-809D419044A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +302,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -374,19 +374,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>28.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>19.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>9.5999999999999961</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -438,22 +438,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,7 +594,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -602,6 +601,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1516,11 +1516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,27 +1560,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>53</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>53</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>53</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>53</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1591,23 +1591,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>44</v>
+        <v>38.4</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>33</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>22</v>
+        <v>19.199999999999996</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>11</v>
+        <v>9.5999999999999961</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="8">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" s="8">
         <v>0</v>
@@ -1871,13 +1871,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
       </c>
       <c r="D16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="8">
         <v>0</v>
@@ -1896,7 +1896,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -1996,13 +1996,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
       </c>
       <c r="D21" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Meeting Recording & Burndown Chart
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBD06AF-A96A-4DB9-94CF-809D419044A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3076CB-3FE8-4FAB-A9EB-368503406B85}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -374,19 +374,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.4</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.799999999999997</c:v>
+                  <c:v>29.400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.199999999999996</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5999999999999961</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -438,22 +438,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>33.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1520,7 +1520,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,27 +1560,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>32.299999999999997</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>32.299999999999997</v>
+        <v>23.25</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>32.299999999999997</v>
+        <v>23.25</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>32.299999999999997</v>
+        <v>23.25</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1591,23 +1591,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>38.4</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>28.799999999999997</v>
+        <v>29.400000000000002</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>19.199999999999996</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>9.5999999999999961</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1771,16 +1771,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
         <v>2</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19" s="8">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>0.2</v>
       </c>
       <c r="E21" s="8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F21" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Burndown & Recording for 20-03 Meeting
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB5C8F1-1BEE-4EB6-8BA2-576028AECCE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80347802-B743-409E-8B9E-0B07A055DB16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -374,19 +374,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>47.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>36.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.5</c:v>
+                  <c:v>27.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>18.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5</c:v>
+                  <c:v>9.0999999999999961</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -438,22 +438,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>47.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.8</c:v>
+                  <c:v>29.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.75</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.75</c:v>
+                  <c:v>13.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.75</c:v>
+                  <c:v>13.59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1520,7 +1520,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,27 +1560,27 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(B7:B38)</f>
-        <v>47.5</v>
+        <v>45.5</v>
       </c>
       <c r="D3" s="2">
         <f>$C3-SUM(C7:C38)</f>
-        <v>45.5</v>
+        <v>43.5</v>
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>31.8</v>
+        <v>29.8</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>21.75</v>
+        <v>19.75</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>21.75</v>
+        <v>13.59</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>21.75</v>
+        <v>13.59</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1591,23 +1591,23 @@
       </c>
       <c r="C4" s="9">
         <f>C3</f>
-        <v>47.5</v>
+        <v>45.5</v>
       </c>
       <c r="D4" s="9">
         <f>C4-$C4/5</f>
-        <v>38</v>
+        <v>36.4</v>
       </c>
       <c r="E4" s="9">
         <f>D4-$C4/5</f>
-        <v>28.5</v>
+        <v>27.299999999999997</v>
       </c>
       <c r="F4" s="9">
         <f>E4-$C4/5</f>
-        <v>19</v>
+        <v>18.199999999999996</v>
       </c>
       <c r="G4" s="9">
         <f>F4-$C4/5</f>
-        <v>9.5</v>
+        <v>9.0999999999999961</v>
       </c>
       <c r="H4" s="9">
         <f>G4-$C4/5</f>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -1833,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="8">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="G20" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Burndown & Quickfire meeting recording
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80347802-B743-409E-8B9E-0B07A055DB16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B05D7D4-4731-4BEA-BE8F-E256E7092C6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
                   <c:v>13.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.59</c:v>
+                  <c:v>6.5900000000000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1520,7 +1520,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>13.59</v>
+        <v>6.5900000000000034</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1786,7 +1786,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1836,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -2011,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>

</xml_diff>